<commit_message>
origin model_2 test results
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes Origin model_2/Curriculum Yes Origin model_2_TEST_HETEROGEINEOUS_TOO_HARD/Curriculum Yes Origin model_2_TEST_HETEROGEINEOUS_TOO_HARD_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes Origin model_2/Curriculum Yes Origin model_2_TEST_HETEROGEINEOUS_TOO_HARD/Curriculum Yes Origin model_2_TEST_HETEROGEINEOUS_TOO_HARD_Test_Result.xlsx
@@ -448,13 +448,13 @@
         <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>